<commit_message>
delete comments legacy comments from mnl example xlsx
</commit_message>
<xml_diff>
--- a/data/mnl/data.xlsx
+++ b/data/mnl/data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdorfner\Documents\Themen\Thesis\Modelle\rivus\data\mnl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kristof\GIT\Masterarbeit\rivus\data\mnl\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="600" yWindow="72" windowWidth="22512" windowHeight="9780" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="Time" sheetId="5" r:id="rId5"/>
     <sheet name="Area-Demand" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="65">
   <si>
     <t>Commodity</t>
   </si>
@@ -280,31 +280,7 @@
     <t>Waste incineration plant</t>
   </si>
   <si>
-    <t>In Richter: GT (gas turbine), DT (steam turbine), so maybe split into two processes as well</t>
-  </si>
-  <si>
-    <t>not mentioned</t>
-  </si>
-  <si>
-    <t>not mendioned</t>
-  </si>
-  <si>
     <t>Waste</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>not mentioned in Richter</t>
-  </si>
-  <si>
-    <t>not mentioned in Richter (interesting: why?)</t>
-  </si>
-  <si>
-    <t>in Richter: BK</t>
-  </si>
-  <si>
-    <t>in Richter: MV</t>
   </si>
   <si>
     <t>t mid</t>
@@ -328,11 +304,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,6 +350,13 @@
       <i/>
       <sz val="11"/>
       <color theme="6" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -509,7 +492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -558,9 +541,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -681,6 +671,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -716,6 +723,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -891,20 +915,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="2.85546875" style="9" customWidth="1"/>
-    <col min="3" max="16384" width="11.42578125" style="9"/>
+    <col min="1" max="2" width="2.88671875" style="9" customWidth="1"/>
+    <col min="3" max="16384" width="11.44140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
@@ -915,7 +939,7 @@
       <c r="I2" s="12"/>
       <c r="J2" s="13"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="14"/>
       <c r="C3" s="15" t="s">
         <v>24</v>
@@ -928,7 +952,7 @@
       <c r="I3" s="16"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="14"/>
       <c r="C4" s="18" t="s">
         <v>47</v>
@@ -941,7 +965,7 @@
       <c r="I4" s="16"/>
       <c r="J4" s="17"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="14"/>
       <c r="C5" s="16"/>
       <c r="D5" s="16"/>
@@ -952,7 +976,7 @@
       <c r="I5" s="16"/>
       <c r="J5" s="17"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="19"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -963,7 +987,7 @@
       <c r="I6" s="10"/>
       <c r="J6" s="20"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="19"/>
       <c r="C7" s="28" t="s">
         <v>44</v>
@@ -976,7 +1000,7 @@
       <c r="I7" s="10"/>
       <c r="J7" s="20"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="19"/>
       <c r="C8" s="26" t="s">
         <v>25</v>
@@ -991,7 +1015,7 @@
       <c r="I8" s="10"/>
       <c r="J8" s="20"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="19"/>
       <c r="C9" s="26" t="s">
         <v>26</v>
@@ -1006,7 +1030,7 @@
       <c r="I9" s="10"/>
       <c r="J9" s="20"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="19"/>
       <c r="C10" s="27" t="s">
         <v>27</v>
@@ -1021,7 +1045,7 @@
       <c r="I10" s="10"/>
       <c r="J10" s="20"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="19"/>
       <c r="C11" s="26" t="s">
         <v>28</v>
@@ -1036,7 +1060,7 @@
       <c r="I11" s="10"/>
       <c r="J11" s="20"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="19"/>
       <c r="C12" s="26" t="s">
         <v>32</v>
@@ -1051,7 +1075,7 @@
       <c r="I12" s="10"/>
       <c r="J12" s="20"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="19"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -1062,7 +1086,7 @@
       <c r="I13" s="10"/>
       <c r="J13" s="20"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="19"/>
       <c r="C14" s="28" t="s">
         <v>45</v>
@@ -1075,7 +1099,7 @@
       <c r="I14" s="10"/>
       <c r="J14" s="20"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="19"/>
       <c r="C15" s="26" t="s">
         <v>29</v>
@@ -1090,7 +1114,7 @@
       <c r="I15" s="10"/>
       <c r="J15" s="20"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="19"/>
       <c r="C16" s="26" t="s">
         <v>30</v>
@@ -1105,7 +1129,7 @@
       <c r="I16" s="10"/>
       <c r="J16" s="20"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="19"/>
       <c r="C17" s="26" t="s">
         <v>31</v>
@@ -1120,7 +1144,7 @@
       <c r="I17" s="10"/>
       <c r="J17" s="20"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="19"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -1131,7 +1155,7 @@
       <c r="I18" s="10"/>
       <c r="J18" s="20"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="19"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -1142,7 +1166,7 @@
       <c r="I19" s="10"/>
       <c r="J19" s="20"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="19"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -1153,7 +1177,7 @@
       <c r="I20" s="10"/>
       <c r="J20" s="20"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="19"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -1164,7 +1188,7 @@
       <c r="I21" s="10"/>
       <c r="J21" s="20"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" s="19"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -1175,7 +1199,7 @@
       <c r="I22" s="10"/>
       <c r="J22" s="20"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" s="19"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -1186,7 +1210,7 @@
       <c r="I23" s="10"/>
       <c r="J23" s="20"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" s="19"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -1197,7 +1221,7 @@
       <c r="I24" s="10"/>
       <c r="J24" s="20"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" s="19"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -1208,7 +1232,7 @@
       <c r="I25" s="10"/>
       <c r="J25" s="20"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="19"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -1219,7 +1243,7 @@
       <c r="I26" s="10"/>
       <c r="J26" s="20"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" s="19"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -1230,7 +1254,7 @@
       <c r="I27" s="10"/>
       <c r="J27" s="20"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" s="21"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
@@ -1248,7 +1272,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1258,18 +1282,18 @@
       <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1"/>
-    <col min="2" max="5" width="11.42578125" style="3"/>
-    <col min="6" max="6" width="11.42578125" style="6"/>
-    <col min="7" max="8" width="11.42578125" style="8"/>
-    <col min="9" max="9" width="11.42578125" style="3"/>
-    <col min="10" max="10" width="12.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="11.44140625" style="1"/>
+    <col min="2" max="5" width="11.44140625" style="3"/>
+    <col min="6" max="6" width="11.44140625" style="6"/>
+    <col min="7" max="8" width="11.44140625" style="8"/>
+    <col min="9" max="9" width="11.44140625" style="3"/>
+    <col min="10" max="10" width="12.5546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.44140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1283,7 +1307,7 @@
         <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>9</v>
@@ -1298,10 +1322,10 @@
         <v>18</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1334,7 +1358,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1367,7 +1391,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1400,7 +1424,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1433,7 +1457,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1469,12 +1493,12 @@
         <v>#N/A</v>
       </c>
       <c r="J6" s="29" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
@@ -1518,26 +1542,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I1:J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="32"/>
-    <col min="3" max="5" width="11.42578125" style="3"/>
-    <col min="6" max="7" width="11.42578125" style="32"/>
-    <col min="8" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="32"/>
+    <col min="3" max="5" width="11.44140625" style="3"/>
+    <col min="6" max="7" width="11.44140625" style="32"/>
+    <col min="8" max="16384" width="11.44140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -1548,7 +1572,7 @@
         <v>16</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>9</v>
@@ -1559,11 +1583,9 @@
       <c r="G1" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="33" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I1" s="33"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -1585,11 +1607,8 @@
       <c r="G2" s="32">
         <v>600000</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
@@ -1611,11 +1630,8 @@
       <c r="G3" s="32">
         <v>600000</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>50</v>
       </c>
@@ -1637,11 +1653,8 @@
       <c r="G4" s="32">
         <v>1000</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>55</v>
       </c>
@@ -1663,11 +1676,8 @@
       <c r="G5" s="32">
         <v>150000</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>53</v>
       </c>
@@ -1689,11 +1699,8 @@
       <c r="G6" s="32">
         <v>400000</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>54</v>
       </c>
@@ -1715,11 +1722,8 @@
       <c r="G7" s="32">
         <v>999990</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>56</v>
       </c>
@@ -1741,11 +1745,8 @@
       <c r="G8" s="32">
         <v>1000</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>57</v>
       </c>
@@ -1767,18 +1768,15 @@
       <c r="G9" s="32">
         <v>0</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>66</v>
-      </c>
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Fixed investment costs (€)" prompt="Up-front investment for building a plant, independent of size._x000a_Has value zero mainly for small-scale technologies." sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Specific investment costs (€/kW)" prompt="Size-dependent part for building a plant." sqref="C1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Variable costs (€/kWh)" prompt="Operational costs to produce one unit of output, excluding fuel costs. Has value zero e.g. for PV or wind turbines (or if no sources are available)." sqref="E1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Minimum capacity (kW)" prompt="Smallest size a plant is typically available in. Has value zero for domestic technologies." sqref="F1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Maximum capacity (kW)" prompt="Biggest capacity a plant typically is available in." sqref="G1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Specific fixed costs (€/kW)" prompt="Size-dependent part for maintaining a plant." sqref="D1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Fixed investment costs (€)" prompt="Up-front investment for building a plant, independent of size._x000a_Has value zero mainly for small-scale technologies." sqref="B1" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Specific investment costs (€/kW)" prompt="Size-dependent part for building a plant." sqref="C1" xr:uid="{00000000-0002-0000-0200-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Variable costs (€/kWh)" prompt="Operational costs to produce one unit of output, excluding fuel costs. Has value zero e.g. for PV or wind turbines (or if no sources are available)." sqref="E1" xr:uid="{00000000-0002-0000-0200-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Minimum capacity (kW)" prompt="Smallest size a plant is typically available in. Has value zero for domestic technologies." sqref="F1" xr:uid="{00000000-0002-0000-0200-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Maximum capacity (kW)" prompt="Biggest capacity a plant typically is available in." sqref="G1" xr:uid="{00000000-0002-0000-0200-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Specific fixed costs (€/kW)" prompt="Size-dependent part for maintaining a plant." sqref="D1" xr:uid="{00000000-0002-0000-0200-000005000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1786,25 +1784,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="D3" sqref="D3:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.42578125" style="1"/>
-    <col min="4" max="4" width="11.42578125" style="6"/>
-    <col min="5" max="16384" width="11.42578125" style="3"/>
+    <col min="2" max="3" width="11.44140625" style="1"/>
+    <col min="4" max="4" width="11.44140625" style="6"/>
+    <col min="5" max="16384" width="11.44140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -1818,7 +1816,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -1832,7 +1830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
@@ -1846,7 +1844,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>51</v>
       </c>
@@ -1860,7 +1858,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>51</v>
       </c>
@@ -1874,7 +1872,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
@@ -1888,7 +1886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>52</v>
       </c>
@@ -1902,7 +1900,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>52</v>
       </c>
@@ -1916,7 +1914,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
@@ -1930,7 +1928,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
@@ -1944,7 +1942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>55</v>
       </c>
@@ -1958,7 +1956,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>50</v>
       </c>
@@ -1972,7 +1970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>50</v>
       </c>
@@ -1986,7 +1984,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>53</v>
       </c>
@@ -2000,7 +1998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>53</v>
       </c>
@@ -2014,7 +2012,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>53</v>
       </c>
@@ -2028,7 +2026,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>54</v>
       </c>
@@ -2042,7 +2040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>54</v>
       </c>
@@ -2056,7 +2054,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>54</v>
       </c>
@@ -2070,7 +2068,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>56</v>
       </c>
@@ -2084,7 +2082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>56</v>
       </c>
@@ -2098,7 +2096,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>56</v>
       </c>
@@ -2112,12 +2110,12 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>12</v>
@@ -2126,7 +2124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>57</v>
       </c>
@@ -2140,7 +2138,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>57</v>
       </c>
@@ -2154,7 +2152,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>57</v>
       </c>
@@ -2192,7 +2190,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Input/output ratio (kWh/kWh)" prompt="Relative power flows in and out of processes. Sum of In and sum of Out should be equal to 1._x000a_For CO2, unit is kg/kWh." sqref="D1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Input/output ratio (kWh/kWh)" prompt="Relative power flows in and out of processes. Sum of In and sum of Out should be equal to 1._x000a_For CO2, unit is kg/kWh." sqref="D1" xr:uid="{00000000-0002-0000-0300-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2219,98 +2217,98 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="3"/>
-    <col min="3" max="3" width="7.85546875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="11.44140625" style="39" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="42"/>
+    <col min="3" max="3" width="7.88671875" style="41" customWidth="1"/>
+    <col min="4" max="4" width="5.109375" style="41" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.44140625" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="38" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="32">
+      <c r="B2" s="40">
         <v>60</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="41">
         <v>1</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="41">
         <v>1</v>
       </c>
-      <c r="E2" s="32"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="32">
+      <c r="E2" s="40"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="40">
         <v>1000</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="41">
         <v>0.8</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="41">
         <v>0.8</v>
       </c>
-      <c r="E3" s="32"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="32">
+      <c r="E3" s="40"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="40">
         <v>2700</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="41">
         <v>0.65</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="41">
         <v>0.65</v>
       </c>
-      <c r="E4" s="32"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="32">
+      <c r="E4" s="40"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="40">
         <v>5000</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="41">
         <v>0.3</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="41">
         <v>0.3</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2319,7 +2317,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2329,14 +2327,14 @@
       <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" style="1"/>
-    <col min="3" max="3" width="11.42578125" style="25"/>
-    <col min="4" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="2" width="11.44140625" style="1"/>
+    <col min="3" max="3" width="11.44140625" style="25"/>
+    <col min="4" max="16384" width="11.44140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>43</v>
       </c>
@@ -2347,7 +2345,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
@@ -2358,7 +2356,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
@@ -2369,7 +2367,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>40</v>
       </c>
@@ -2380,7 +2378,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>40</v>
       </c>
@@ -2391,7 +2389,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
@@ -2402,7 +2400,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -2413,7 +2411,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
@@ -2424,7 +2422,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>42</v>
       </c>

</xml_diff>